<commit_message>
Auto classes, improved snake output.
</commit_message>
<xml_diff>
--- a/Gimmix/src/geneticEmblem/units/factory/FE.xlsx
+++ b/Gimmix/src/geneticEmblem/units/factory/FE.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="127">
   <si>
     <t>Class</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Kaiser</t>
   </si>
   <si>
-    <t>KilnFiend</t>
-  </si>
-  <si>
     <t>Mercedes</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>Regenerate</t>
   </si>
   <si>
-    <t>Flame Wizard</t>
-  </si>
-  <si>
     <t>Monk</t>
   </si>
   <si>
@@ -373,6 +367,51 @@
   </si>
   <si>
     <t>Saracen</t>
+  </si>
+  <si>
+    <t>Cremator</t>
+  </si>
+  <si>
+    <t>Woodcutter</t>
+  </si>
+  <si>
+    <t>Refector Mage</t>
+  </si>
+  <si>
+    <t>Nobles</t>
+  </si>
+  <si>
+    <t>ancemaster</t>
+  </si>
+  <si>
+    <t>Blue Mage</t>
+  </si>
+  <si>
+    <t>Jett</t>
+  </si>
+  <si>
+    <t>Markman</t>
+  </si>
+  <si>
+    <t>Kiln Fiend</t>
+  </si>
+  <si>
+    <t>Explorer</t>
+  </si>
+  <si>
+    <t>Channeler</t>
+  </si>
+  <si>
+    <t>Glem</t>
+  </si>
+  <si>
+    <t>Bandit</t>
+  </si>
+  <si>
+    <t>Viera</t>
+  </si>
+  <si>
+    <t>Butcher</t>
   </si>
 </sst>
 </file>
@@ -486,7 +525,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -585,16 +624,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -645,86 +674,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1658,25 +1607,25 @@
     <sortCondition descending="1" ref="D2:D30"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1690,8 +1639,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1725,14 +1674,14 @@
     </row>
     <row r="2" spans="2:7">
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D2" s="1">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="E2">
-        <f>SUM((100*D2)/2048)</f>
-        <v>8.7890625</v>
+        <f t="shared" ref="E2:E45" si="0">SUM((100*D2)/2048)</f>
+        <v>7.080078125</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -1740,38 +1689,38 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E3">
-        <f>SUM((100*D3)/2048)</f>
-        <v>8.056640625</v>
+        <f t="shared" si="0"/>
+        <v>6.689453125</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E4">
-        <f>SUM((100*D4)/2048)</f>
-        <v>5.6640625</v>
+        <f t="shared" si="0"/>
+        <v>5.078125</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E5">
-        <f>SUM((100*D5)/2048)</f>
-        <v>5.126953125</v>
+        <f t="shared" si="0"/>
+        <v>4.6875</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -1779,146 +1728,146 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E6">
-        <f>SUM((100*D6)/2048)</f>
-        <v>5.126953125</v>
+        <f t="shared" si="0"/>
+        <v>4.443359375</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E7">
-        <f>SUM((100*D7)/2048)</f>
-        <v>4.443359375</v>
+        <f t="shared" si="0"/>
+        <v>4.345703125</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="C8" s="1" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="D8" s="1">
         <v>80</v>
       </c>
       <c r="E8">
-        <f>SUM((100*D8)/2048)</f>
+        <f t="shared" si="0"/>
         <v>3.90625</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E9">
-        <f>SUM((100*D9)/2048)</f>
-        <v>3.857421875</v>
+        <f t="shared" si="0"/>
+        <v>3.662109375</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D10" s="1">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E10">
-        <f>SUM((100*D10)/2048)</f>
-        <v>3.80859375</v>
+        <f t="shared" si="0"/>
+        <v>3.515625</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="D11" s="1">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E11">
-        <f>SUM((100*D11)/2048)</f>
-        <v>3.759765625</v>
+        <f t="shared" si="0"/>
+        <v>3.466796875</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="C12" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D12" s="1">
         <v>66</v>
       </c>
       <c r="E12">
-        <f>SUM((100*D12)/2048)</f>
+        <f t="shared" si="0"/>
         <v>3.22265625</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13">
-        <f>SUM((100*D13)/2048)</f>
-        <v>3.173828125</v>
+        <f t="shared" si="0"/>
+        <v>3.22265625</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E14">
-        <f>SUM((100*D14)/2048)</f>
-        <v>3.076171875</v>
+        <f t="shared" si="0"/>
+        <v>3.173828125</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E15">
-        <f>SUM((100*D15)/2048)</f>
-        <v>2.734375</v>
+        <f t="shared" si="0"/>
+        <v>3.125</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E16">
-        <f>SUM((100*D16)/2048)</f>
-        <v>2.685546875</v>
+        <f t="shared" si="0"/>
+        <v>2.9296875</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="D17" s="1">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E17">
-        <f>SUM((100*D17)/2048)</f>
-        <v>2.587890625</v>
+        <f t="shared" si="0"/>
+        <v>2.734375</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -1926,26 +1875,26 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="D18" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E18">
-        <f>SUM((100*D18)/2048)</f>
-        <v>2.587890625</v>
+        <f t="shared" si="0"/>
+        <v>2.685546875</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E19">
-        <f>SUM((100*D19)/2048)</f>
-        <v>2.5390625</v>
+        <f t="shared" si="0"/>
+        <v>2.63671875</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>15</v>
@@ -1957,50 +1906,50 @@
     </row>
     <row r="20" spans="2:8">
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="D20" s="1">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E20">
-        <f>SUM((100*D20)/2048)</f>
-        <v>2.34375</v>
+        <f t="shared" si="0"/>
+        <v>2.44140625</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E21">
-        <f>SUM((100*D21)/2048)</f>
-        <v>2.34375</v>
+        <f t="shared" si="0"/>
+        <v>2.392578125</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E22">
-        <f>SUM((100*D22)/2048)</f>
-        <v>2.1484375</v>
+        <f t="shared" si="0"/>
+        <v>2.197265625</v>
       </c>
     </row>
     <row r="23" spans="2:8">
       <c r="C23" s="1" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23">
-        <f>SUM((100*D23)/2048)</f>
-        <v>2.1484375</v>
+        <f t="shared" si="0"/>
+        <v>2.099609375</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -2008,166 +1957,262 @@
         <v>44</v>
       </c>
       <c r="D24" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E24">
-        <f>SUM((100*D24)/2048)</f>
-        <v>1.904296875</v>
+        <f t="shared" si="0"/>
+        <v>2.05078125</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D25" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25">
-        <f>SUM((100*D25)/2048)</f>
-        <v>1.85546875</v>
+        <f t="shared" si="0"/>
+        <v>1.953125</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="C26" s="1" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E26">
-        <f>SUM((100*D26)/2048)</f>
-        <v>1.7578125</v>
+        <f t="shared" si="0"/>
+        <v>1.904296875</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="D27" s="1">
         <v>35</v>
       </c>
       <c r="E27">
-        <f>SUM((100*D27)/2048)</f>
+        <f t="shared" si="0"/>
         <v>1.708984375</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="D28" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28">
-        <f>SUM((100*D28)/2048)</f>
-        <v>1.66015625</v>
+        <f t="shared" si="0"/>
+        <v>1.611328125</v>
       </c>
     </row>
     <row r="29" spans="2:8">
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="D29" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29">
-        <f>SUM((100*D29)/2048)</f>
-        <v>1.46484375</v>
+        <f t="shared" si="0"/>
+        <v>1.513671875</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="C30" s="1" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1">
         <v>28</v>
       </c>
       <c r="E30">
-        <f>SUM((100*D30)/2048)</f>
+        <f t="shared" si="0"/>
         <v>1.3671875</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31">
-        <f>SUM((100*D31)/2048)</f>
-        <v>1.220703125</v>
+        <f t="shared" si="0"/>
+        <v>1.171875</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="C32" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D32" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32">
-        <f>SUM((100*D32)/2048)</f>
-        <v>1.220703125</v>
+        <f t="shared" si="0"/>
+        <v>1.171875</v>
       </c>
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="D33" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E33">
-        <f>SUM((100*D33)/2048)</f>
-        <v>0.830078125</v>
+        <f t="shared" si="0"/>
+        <v>1.07421875</v>
       </c>
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D34" s="1">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E34">
-        <f>SUM((100*D34)/2048)</f>
-        <v>0.5859375</v>
+        <f t="shared" si="0"/>
+        <v>1.025390625</v>
       </c>
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="1" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D35" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E35">
-        <f>SUM((100*D35)/2048)</f>
-        <v>0.146484375</v>
+        <f t="shared" si="0"/>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="36" spans="3:6">
       <c r="C36" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E36">
-        <f>SUM((100*D36)/2048)</f>
-        <v>9.765625E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D37" s="1">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0.537109375</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="1">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.439453125</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6">
+      <c r="C39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.439453125</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="1">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0.439453125</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>9.765625E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6">
+      <c r="C42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E37">
-        <f>SUM((100*D37)/2048)</f>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>4.8828125E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>4.8828125E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>4.8828125E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
         <v>4.8828125E-2</v>
       </c>
     </row>
@@ -2186,7 +2231,7 @@
     <sortCondition ref="C10:C45"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2434,21 +2479,21 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>81</v>
@@ -2456,10 +2501,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>82</v>
@@ -2467,10 +2512,10 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>84</v>
@@ -2478,10 +2523,10 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>83</v>

</xml_diff>